<commit_message>
MAJ input file : node 19 added
</commit_message>
<xml_diff>
--- a/grid_data_input_file_building_demo.xlsx
+++ b/grid_data_input_file_building_demo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c30483\Documents\dc_design_tool\dc_design_tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I43680\Documents\pythonProjects\dc_design_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE60663-DEF1-405D-923E-D040E6942DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7F6992-AFD6-4A50-9E39-C8010888F839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SLD Building" sheetId="13" r:id="rId1"/>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="357">
   <si>
     <t>Node_i</t>
   </si>
@@ -1419,6 +1419,9 @@
   <si>
     <t>[1.2; 1], [1.005; 0.0], [1.0; 0], [1; 0], [0.995;0], [0.8; -1]</t>
   </si>
+  <si>
+    <t>Profile of node 19</t>
+  </si>
 </sst>
 </file>
 
@@ -1954,29 +1957,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
@@ -1990,29 +1987,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2022,6 +2016,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2101,23 +2104,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>625856</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>143443</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>95671</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>99597</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="704" name="Image 703">
+        <xdr:cNvPr id="2" name="Image 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EC8ADD1-F290-B94A-A741-80BE96F4C555}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98146C6D-D129-23C1-E2BD-0D989CAF986E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2133,8 +2136,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="904875" y="276225"/>
-          <a:ext cx="11722481" cy="6553768"/>
+          <a:off x="3396343" y="1567543"/>
+          <a:ext cx="11133785" cy="6195597"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2204,23 +2207,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>251046</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>20373</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>397565</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>83133</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>327273</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>41069</xdr:rowOff>
+      <xdr:colOff>386271</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>145980</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
+        <xdr:cNvPr id="3" name="Image 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E72832F-BC45-4C0A-B6B1-094C85BDAF99}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74918CD1-F5BF-5F46-7D21-E6C404AED6CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2236,8 +2239,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4682242" y="2463743"/>
-          <a:ext cx="7514009" cy="4195130"/>
+          <a:off x="3472069" y="2157098"/>
+          <a:ext cx="8781524" cy="4886639"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2253,23 +2256,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>626746</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>126091</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1314451</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>17712</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>176225</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>61497</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
+        <xdr:cNvPr id="3" name="Image 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E69C2B51-5AB3-407F-80C3-99E860393B2C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{311764A5-2781-E993-9CF1-CCDF83E8147B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2285,8 +2288,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3627121" y="2012041"/>
-          <a:ext cx="10260330" cy="5720921"/>
+          <a:off x="7871460" y="2804160"/>
+          <a:ext cx="11133785" cy="6195597"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2303,22 +2306,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>248666</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>135823</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>275285</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>8157</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
+        <xdr:cNvPr id="3" name="Image 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F7B66DA-26F7-475A-B268-D25BFEF9D1A5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAF3A687-D4D0-0BC9-F7AD-923DD3F51D9C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2334,8 +2337,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4143375" y="276225"/>
-          <a:ext cx="11726291" cy="6553768"/>
+          <a:off x="4038600" y="1173480"/>
+          <a:ext cx="11133785" cy="6195597"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2651,7 +2654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC5D1895-B990-4AED-BF1D-6215F7A4F79E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -2669,8 +2672,8 @@
   </sheetPr>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3654,16 +3657,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="40"/>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
       <c r="D1" s="40"/>
     </row>
     <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="40"/>
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="102" t="s">
         <v>256</v>
       </c>
-      <c r="C2" s="104"/>
+      <c r="C2" s="102"/>
       <c r="D2" s="40"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3672,18 +3675,18 @@
     </row>
     <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="40"/>
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="101" t="s">
         <v>243</v>
       </c>
-      <c r="C4" s="103"/>
+      <c r="C4" s="101"/>
       <c r="D4" s="40"/>
     </row>
     <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="40"/>
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="100" t="s">
         <v>244</v>
       </c>
-      <c r="C5" s="102"/>
+      <c r="C5" s="100"/>
       <c r="D5" s="40"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3696,70 +3699,70 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="40"/>
-      <c r="B8" s="95" t="s">
+      <c r="B8" s="107" t="s">
         <v>213</v>
       </c>
-      <c r="C8" s="95"/>
+      <c r="C8" s="107"/>
       <c r="D8" s="40"/>
     </row>
     <row r="9" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="40"/>
-      <c r="B9" s="105" t="s">
+      <c r="B9" s="103" t="s">
         <v>212</v>
       </c>
-      <c r="C9" s="105"/>
+      <c r="C9" s="103"/>
       <c r="D9" s="40"/>
     </row>
     <row r="10" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="40"/>
-      <c r="B10" s="105" t="s">
+      <c r="B10" s="103" t="s">
         <v>211</v>
       </c>
-      <c r="C10" s="105"/>
+      <c r="C10" s="103"/>
       <c r="D10" s="40"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="40"/>
-      <c r="B11" s="96" t="s">
+      <c r="B11" s="104" t="s">
         <v>215</v>
       </c>
-      <c r="C11" s="96"/>
+      <c r="C11" s="104"/>
       <c r="D11" s="40"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="40"/>
-      <c r="B12" s="105" t="s">
+      <c r="B12" s="103" t="s">
         <v>216</v>
       </c>
-      <c r="C12" s="105"/>
+      <c r="C12" s="103"/>
       <c r="D12" s="40"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="40"/>
-      <c r="B13" s="97" t="s">
+      <c r="B13" s="94" t="s">
         <v>217</v>
       </c>
-      <c r="C13" s="97"/>
+      <c r="C13" s="94"/>
       <c r="D13" s="45"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="40"/>
-      <c r="B14" s="97"/>
-      <c r="C14" s="97"/>
+      <c r="B14" s="94"/>
+      <c r="C14" s="94"/>
       <c r="D14" s="46"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="40"/>
-      <c r="B15" s="97"/>
-      <c r="C15" s="97"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="94"/>
       <c r="D15" s="40"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="40"/>
-      <c r="B16" s="95" t="s">
+      <c r="B16" s="107" t="s">
         <v>214</v>
       </c>
-      <c r="C16" s="95"/>
+      <c r="C16" s="107"/>
       <c r="D16" s="47"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3830,18 +3833,18 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="40"/>
-      <c r="B24" s="96" t="s">
+      <c r="B24" s="104" t="s">
         <v>288</v>
       </c>
-      <c r="C24" s="96"/>
+      <c r="C24" s="104"/>
       <c r="D24" s="40"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="40"/>
-      <c r="B25" s="97" t="s">
+      <c r="B25" s="94" t="s">
         <v>289</v>
       </c>
-      <c r="C25" s="97"/>
+      <c r="C25" s="94"/>
       <c r="D25" s="40"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3870,24 +3873,24 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="40"/>
-      <c r="B29" s="97" t="s">
+      <c r="B29" s="94" t="s">
         <v>293</v>
       </c>
-      <c r="C29" s="97"/>
+      <c r="C29" s="94"/>
       <c r="D29" s="40"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="40"/>
-      <c r="B30" s="106" t="s">
+      <c r="B30" s="105" t="s">
         <v>294</v>
       </c>
-      <c r="C30" s="106"/>
+      <c r="C30" s="105"/>
       <c r="D30" s="40"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="40"/>
-      <c r="B31" s="97"/>
-      <c r="C31" s="97"/>
+      <c r="B31" s="94"/>
+      <c r="C31" s="94"/>
       <c r="D31" s="40"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3900,42 +3903,42 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="40"/>
-      <c r="B33" s="100" t="s">
+      <c r="B33" s="99" t="s">
         <v>221</v>
       </c>
-      <c r="C33" s="100"/>
+      <c r="C33" s="99"/>
       <c r="D33" s="40"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="40"/>
-      <c r="B34" s="97" t="s">
+      <c r="B34" s="94" t="s">
         <v>220</v>
       </c>
-      <c r="C34" s="97"/>
+      <c r="C34" s="94"/>
       <c r="D34" s="40"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="40"/>
-      <c r="B35" s="108" t="s">
+      <c r="B35" s="96" t="s">
         <v>219</v>
       </c>
-      <c r="C35" s="108"/>
+      <c r="C35" s="96"/>
       <c r="D35" s="40"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="40"/>
-      <c r="B36" s="107" t="s">
+      <c r="B36" s="95" t="s">
         <v>223</v>
       </c>
-      <c r="C36" s="107"/>
+      <c r="C36" s="95"/>
       <c r="D36" s="40"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="40"/>
-      <c r="B37" s="97" t="s">
+      <c r="B37" s="94" t="s">
         <v>245</v>
       </c>
-      <c r="C37" s="97"/>
+      <c r="C37" s="94"/>
       <c r="D37" s="40"/>
       <c r="F37" t="s">
         <v>242</v>
@@ -3943,26 +3946,26 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="40"/>
-      <c r="B38" s="97" t="s">
+      <c r="B38" s="94" t="s">
         <v>246</v>
       </c>
-      <c r="C38" s="97"/>
+      <c r="C38" s="94"/>
       <c r="D38" s="40"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="40"/>
-      <c r="B39" s="108" t="s">
+      <c r="B39" s="96" t="s">
         <v>247</v>
       </c>
-      <c r="C39" s="108"/>
+      <c r="C39" s="96"/>
       <c r="D39" s="40"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="40"/>
-      <c r="B40" s="97" t="s">
+      <c r="B40" s="94" t="s">
         <v>248</v>
       </c>
-      <c r="C40" s="97"/>
+      <c r="C40" s="94"/>
       <c r="D40" s="40"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -3971,190 +3974,190 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="40"/>
-      <c r="B42" s="100" t="s">
+      <c r="B42" s="99" t="s">
         <v>258</v>
       </c>
-      <c r="C42" s="100"/>
+      <c r="C42" s="99"/>
       <c r="D42" s="40"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="40"/>
-      <c r="B43" s="97" t="s">
+      <c r="B43" s="94" t="s">
         <v>222</v>
       </c>
-      <c r="C43" s="97"/>
+      <c r="C43" s="94"/>
       <c r="D43" s="40"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="40"/>
-      <c r="B44" s="97" t="s">
+      <c r="B44" s="94" t="s">
         <v>249</v>
       </c>
-      <c r="C44" s="97"/>
+      <c r="C44" s="94"/>
       <c r="D44" s="40"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="40"/>
-      <c r="B45" s="97" t="s">
+      <c r="B45" s="94" t="s">
         <v>250</v>
       </c>
-      <c r="C45" s="97"/>
+      <c r="C45" s="94"/>
       <c r="D45" s="40"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="40"/>
-      <c r="B46" s="97" t="s">
+      <c r="B46" s="94" t="s">
         <v>251</v>
       </c>
-      <c r="C46" s="97"/>
+      <c r="C46" s="94"/>
       <c r="D46" s="40"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="40"/>
-      <c r="B47" s="98" t="s">
+      <c r="B47" s="108" t="s">
         <v>224</v>
       </c>
-      <c r="C47" s="98"/>
+      <c r="C47" s="108"/>
       <c r="D47" s="40"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="40"/>
-      <c r="B48" s="97" t="s">
+      <c r="B48" s="94" t="s">
         <v>225</v>
       </c>
-      <c r="C48" s="97"/>
+      <c r="C48" s="94"/>
       <c r="D48" s="40"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="40"/>
-      <c r="B49" s="97" t="s">
+      <c r="B49" s="94" t="s">
         <v>226</v>
       </c>
-      <c r="C49" s="97"/>
+      <c r="C49" s="94"/>
       <c r="D49" s="40"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="40"/>
-      <c r="B50" s="97" t="s">
+      <c r="B50" s="94" t="s">
         <v>227</v>
       </c>
-      <c r="C50" s="97"/>
+      <c r="C50" s="94"/>
       <c r="D50" s="40"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="40"/>
-      <c r="B51" s="97"/>
-      <c r="C51" s="97"/>
+      <c r="B51" s="94"/>
+      <c r="C51" s="94"/>
       <c r="D51" s="40"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="40"/>
-      <c r="B52" s="100" t="s">
+      <c r="B52" s="99" t="s">
         <v>228</v>
       </c>
-      <c r="C52" s="100"/>
+      <c r="C52" s="99"/>
       <c r="D52" s="40"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="40"/>
-      <c r="B53" s="97" t="s">
+      <c r="B53" s="94" t="s">
         <v>229</v>
       </c>
-      <c r="C53" s="97"/>
+      <c r="C53" s="94"/>
       <c r="D53" s="40"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="40"/>
-      <c r="B54" s="99" t="s">
+      <c r="B54" s="97" t="s">
         <v>252</v>
       </c>
-      <c r="C54" s="97"/>
+      <c r="C54" s="94"/>
       <c r="D54" s="40"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="40"/>
-      <c r="B55" s="97" t="s">
+      <c r="B55" s="94" t="s">
         <v>233</v>
       </c>
-      <c r="C55" s="97"/>
+      <c r="C55" s="94"/>
       <c r="D55" s="40"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="40"/>
-      <c r="B56" s="99" t="s">
+      <c r="B56" s="97" t="s">
         <v>253</v>
       </c>
-      <c r="C56" s="97"/>
+      <c r="C56" s="94"/>
       <c r="D56" s="40"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="40"/>
-      <c r="B57" s="97" t="s">
+      <c r="B57" s="94" t="s">
         <v>232</v>
       </c>
-      <c r="C57" s="97"/>
+      <c r="C57" s="94"/>
       <c r="D57" s="40"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="40"/>
-      <c r="B58" s="99" t="s">
+      <c r="B58" s="97" t="s">
         <v>254</v>
       </c>
-      <c r="C58" s="97"/>
+      <c r="C58" s="94"/>
       <c r="D58" s="40"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="40"/>
-      <c r="B59" s="97" t="s">
+      <c r="B59" s="94" t="s">
         <v>231</v>
       </c>
-      <c r="C59" s="97"/>
+      <c r="C59" s="94"/>
       <c r="D59" s="40"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="40"/>
-      <c r="B60" s="99" t="s">
+      <c r="B60" s="97" t="s">
         <v>255</v>
       </c>
-      <c r="C60" s="97"/>
+      <c r="C60" s="94"/>
       <c r="D60" s="40"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="40"/>
-      <c r="B61" s="97" t="s">
+      <c r="B61" s="94" t="s">
         <v>230</v>
       </c>
-      <c r="C61" s="97"/>
+      <c r="C61" s="94"/>
       <c r="D61" s="40"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="40"/>
-      <c r="B62" s="97"/>
-      <c r="C62" s="97"/>
+      <c r="B62" s="94"/>
+      <c r="C62" s="94"/>
       <c r="D62" s="40"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="40"/>
-      <c r="B63" s="100" t="s">
+      <c r="B63" s="99" t="s">
         <v>239</v>
       </c>
-      <c r="C63" s="100"/>
+      <c r="C63" s="99"/>
       <c r="D63" s="40"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="40"/>
-      <c r="B64" s="97" t="s">
+      <c r="B64" s="94" t="s">
         <v>240</v>
       </c>
-      <c r="C64" s="97"/>
+      <c r="C64" s="94"/>
       <c r="D64" s="40"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="40"/>
-      <c r="B65" s="97" t="s">
+      <c r="B65" s="94" t="s">
         <v>241</v>
       </c>
-      <c r="C65" s="97"/>
+      <c r="C65" s="94"/>
       <c r="D65" s="40"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -4165,69 +4168,112 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="40"/>
-      <c r="B67" s="97"/>
-      <c r="C67" s="97"/>
+      <c r="B67" s="94"/>
+      <c r="C67" s="94"/>
       <c r="D67" s="40"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="40"/>
-      <c r="B68" s="100" t="s">
+      <c r="B68" s="99" t="s">
         <v>238</v>
       </c>
-      <c r="C68" s="100"/>
+      <c r="C68" s="99"/>
       <c r="D68" s="40"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="40"/>
-      <c r="B69" s="97" t="s">
+      <c r="B69" s="94" t="s">
         <v>234</v>
       </c>
-      <c r="C69" s="97"/>
+      <c r="C69" s="94"/>
       <c r="D69" s="40"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="40"/>
-      <c r="B70" s="97" t="s">
+      <c r="B70" s="94" t="s">
         <v>235</v>
       </c>
-      <c r="C70" s="97"/>
+      <c r="C70" s="94"/>
       <c r="D70" s="40"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="40"/>
-      <c r="B71" s="97" t="s">
+      <c r="B71" s="94" t="s">
         <v>236</v>
       </c>
-      <c r="C71" s="97"/>
+      <c r="C71" s="94"/>
       <c r="D71" s="40"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="40"/>
-      <c r="B72" s="97" t="s">
+      <c r="B72" s="94" t="s">
         <v>237</v>
       </c>
-      <c r="C72" s="97"/>
+      <c r="C72" s="94"/>
       <c r="D72" s="40"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="40"/>
-      <c r="B73" s="94"/>
-      <c r="C73" s="94"/>
+      <c r="B73" s="106"/>
+      <c r="C73" s="106"/>
       <c r="D73" s="40"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B74" s="44"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="97"/>
-      <c r="C77" s="97"/>
+      <c r="B77" s="94"/>
+      <c r="C77" s="94"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="97"/>
-      <c r="C78" s="97"/>
+      <c r="B78" s="94"/>
+      <c r="C78" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="59">
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B30:C30"/>
     <mergeCell ref="B77:C77"/>
     <mergeCell ref="B78:C78"/>
     <mergeCell ref="B36:C36"/>
@@ -4244,49 +4290,6 @@
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4323,15 +4326,15 @@
   <sheetData>
     <row r="1" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="49"/>
-      <c r="B1" s="113" t="s">
+      <c r="B1" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
       <c r="I1" s="49"/>
     </row>
     <row r="2" spans="1:9" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4412,7 +4415,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="31"/>
-      <c r="G5" s="111"/>
+      <c r="G5" s="110"/>
       <c r="H5" s="17"/>
       <c r="I5" s="49"/>
     </row>
@@ -4444,7 +4447,7 @@
       <c r="E7" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="G7" s="97"/>
+      <c r="G7" s="94"/>
       <c r="I7" s="49"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -4452,7 +4455,7 @@
       <c r="E8" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="G8" s="97"/>
+      <c r="G8" s="94"/>
       <c r="I8" s="49"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -4464,7 +4467,7 @@
         <v>104</v>
       </c>
       <c r="F9" s="31"/>
-      <c r="G9" s="111"/>
+      <c r="G9" s="110"/>
       <c r="H9" s="17"/>
       <c r="I9" s="49"/>
     </row>
@@ -4495,12 +4498,12 @@
       <c r="A11" s="49"/>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
-      <c r="D11" s="111"/>
+      <c r="D11" s="110"/>
       <c r="E11" s="18" t="s">
         <v>257</v>
       </c>
       <c r="F11" s="31"/>
-      <c r="G11" s="111"/>
+      <c r="G11" s="110"/>
       <c r="H11" s="17"/>
       <c r="I11" s="49"/>
     </row>
@@ -4532,7 +4535,7 @@
       <c r="E13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="97"/>
+      <c r="G13" s="94"/>
       <c r="I13" s="49"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -4544,7 +4547,7 @@
         <v>22</v>
       </c>
       <c r="F14" s="31"/>
-      <c r="G14" s="111"/>
+      <c r="G14" s="110"/>
       <c r="H14" s="17"/>
       <c r="I14" s="49"/>
     </row>
@@ -4800,7 +4803,7 @@
         <v>99</v>
       </c>
       <c r="F26" s="31"/>
-      <c r="G26" s="111"/>
+      <c r="G26" s="110"/>
       <c r="H26" s="17"/>
       <c r="I26" s="49"/>
       <c r="K26" s="4"/>
@@ -4840,7 +4843,7 @@
         <v>101</v>
       </c>
       <c r="F28" s="31"/>
-      <c r="G28" s="111"/>
+      <c r="G28" s="110"/>
       <c r="H28" s="17"/>
       <c r="I28" s="49"/>
       <c r="K28" s="4"/>
@@ -4880,7 +4883,7 @@
       <c r="F30" s="32" t="s">
         <v>190</v>
       </c>
-      <c r="G30" s="111"/>
+      <c r="G30" s="110"/>
       <c r="I30" s="49"/>
       <c r="K30" s="4"/>
       <c r="M30" s="4"/>
@@ -5088,7 +5091,7 @@
         <v>10</v>
       </c>
       <c r="F41" s="84"/>
-      <c r="G41" s="110"/>
+      <c r="G41" s="114"/>
       <c r="H41" s="56"/>
       <c r="I41" s="49"/>
       <c r="K41" s="4"/>
@@ -5103,7 +5106,7 @@
         <v>15</v>
       </c>
       <c r="F42" s="84"/>
-      <c r="G42" s="110"/>
+      <c r="G42" s="114"/>
       <c r="H42" s="56"/>
       <c r="I42" s="49"/>
       <c r="K42" s="4"/>
@@ -5118,7 +5121,7 @@
         <v>20</v>
       </c>
       <c r="F43" s="84"/>
-      <c r="G43" s="110"/>
+      <c r="G43" s="114"/>
       <c r="H43" s="56"/>
       <c r="I43" s="49"/>
       <c r="K43" s="4"/>
@@ -5133,7 +5136,7 @@
         <v>30</v>
       </c>
       <c r="F44" s="84"/>
-      <c r="G44" s="110"/>
+      <c r="G44" s="114"/>
       <c r="H44" s="56"/>
       <c r="I44" s="49"/>
       <c r="K44" s="4"/>
@@ -5148,7 +5151,7 @@
         <v>60</v>
       </c>
       <c r="F45" s="31"/>
-      <c r="G45" s="111"/>
+      <c r="G45" s="110"/>
       <c r="H45" s="17"/>
       <c r="I45" s="49"/>
       <c r="K45" s="4"/>
@@ -5195,7 +5198,7 @@
       <c r="F47" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="G47" s="116" t="s">
+      <c r="G47" s="113" t="s">
         <v>185</v>
       </c>
       <c r="H47" s="25"/>
@@ -5206,7 +5209,7 @@
       <c r="E48" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G48" s="97"/>
+      <c r="G48" s="94"/>
       <c r="I48" s="49"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -5214,7 +5217,7 @@
       <c r="E49" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G49" s="97"/>
+      <c r="G49" s="94"/>
       <c r="I49" s="49"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -5222,7 +5225,7 @@
       <c r="E50" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G50" s="97"/>
+      <c r="G50" s="94"/>
       <c r="I50" s="49"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -5230,7 +5233,7 @@
       <c r="E51" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G51" s="97"/>
+      <c r="G51" s="94"/>
       <c r="I51" s="49"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -5242,7 +5245,7 @@
         <v>24</v>
       </c>
       <c r="F52" s="31"/>
-      <c r="G52" s="111"/>
+      <c r="G52" s="110"/>
       <c r="H52" s="17"/>
       <c r="I52" s="49"/>
     </row>
@@ -5298,7 +5301,7 @@
       <c r="F55" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="G55" s="97"/>
+      <c r="G55" s="94"/>
       <c r="I55" s="49"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -5309,7 +5312,7 @@
       <c r="F56" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="G56" s="97"/>
+      <c r="G56" s="94"/>
       <c r="I56" s="49"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -5323,7 +5326,7 @@
       <c r="F57" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="G57" s="111"/>
+      <c r="G57" s="110"/>
       <c r="H57" s="17"/>
       <c r="I57" s="49"/>
     </row>
@@ -5545,7 +5548,7 @@
         <v>115</v>
       </c>
       <c r="F69" s="84"/>
-      <c r="G69" s="110"/>
+      <c r="G69" s="114"/>
       <c r="H69" s="56"/>
       <c r="I69" s="49"/>
     </row>
@@ -5558,7 +5561,7 @@
         <v>323</v>
       </c>
       <c r="F70" s="84"/>
-      <c r="G70" s="110"/>
+      <c r="G70" s="114"/>
       <c r="H70" s="56"/>
       <c r="I70" s="49"/>
     </row>
@@ -5571,7 +5574,7 @@
         <v>324</v>
       </c>
       <c r="F71" s="84"/>
-      <c r="G71" s="110"/>
+      <c r="G71" s="114"/>
       <c r="H71" s="56"/>
       <c r="I71" s="49"/>
     </row>
@@ -5584,7 +5587,7 @@
         <v>327</v>
       </c>
       <c r="F72" s="84"/>
-      <c r="G72" s="110"/>
+      <c r="G72" s="114"/>
       <c r="H72" s="56"/>
       <c r="I72" s="49"/>
     </row>
@@ -5597,7 +5600,7 @@
         <v>329</v>
       </c>
       <c r="F73" s="84"/>
-      <c r="G73" s="110"/>
+      <c r="G73" s="114"/>
       <c r="H73" s="56"/>
       <c r="I73" s="49"/>
     </row>
@@ -5610,7 +5613,7 @@
         <v>328</v>
       </c>
       <c r="F74" s="84"/>
-      <c r="G74" s="110"/>
+      <c r="G74" s="114"/>
       <c r="H74" s="56"/>
       <c r="I74" s="49"/>
     </row>
@@ -5623,7 +5626,7 @@
         <v>325</v>
       </c>
       <c r="F75" s="84"/>
-      <c r="G75" s="110"/>
+      <c r="G75" s="114"/>
       <c r="H75" s="56"/>
       <c r="I75" s="49"/>
     </row>
@@ -5636,7 +5639,7 @@
         <v>339</v>
       </c>
       <c r="F76" s="84"/>
-      <c r="G76" s="110"/>
+      <c r="G76" s="114"/>
       <c r="H76" s="56"/>
       <c r="I76" s="49"/>
     </row>
@@ -5649,7 +5652,7 @@
         <v>338</v>
       </c>
       <c r="F77" s="84"/>
-      <c r="G77" s="110"/>
+      <c r="G77" s="114"/>
       <c r="H77" s="56"/>
       <c r="I77" s="49"/>
     </row>
@@ -5662,7 +5665,7 @@
         <v>326</v>
       </c>
       <c r="F78" s="84"/>
-      <c r="G78" s="110"/>
+      <c r="G78" s="114"/>
       <c r="H78" s="56"/>
       <c r="I78" s="49"/>
     </row>
@@ -5675,7 +5678,7 @@
         <v>337</v>
       </c>
       <c r="F79" s="84"/>
-      <c r="G79" s="110"/>
+      <c r="G79" s="114"/>
       <c r="H79" s="56"/>
       <c r="I79" s="49"/>
     </row>
@@ -5688,7 +5691,7 @@
         <v>340</v>
       </c>
       <c r="F80" s="86"/>
-      <c r="G80" s="112"/>
+      <c r="G80" s="115"/>
       <c r="H80" s="87"/>
       <c r="I80" s="49"/>
     </row>
@@ -5783,7 +5786,7 @@
       <c r="E85" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="G85" s="97"/>
+      <c r="G85" s="94"/>
       <c r="I85" s="49"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -5791,7 +5794,7 @@
       <c r="E86" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G86" s="97"/>
+      <c r="G86" s="94"/>
       <c r="I86" s="49"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -5799,7 +5802,7 @@
       <c r="E87" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="G87" s="97"/>
+      <c r="G87" s="94"/>
       <c r="I87" s="49"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -5807,7 +5810,7 @@
       <c r="E88" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="G88" s="97"/>
+      <c r="G88" s="94"/>
       <c r="I88" s="49"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -5815,7 +5818,7 @@
       <c r="E89" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G89" s="97"/>
+      <c r="G89" s="94"/>
       <c r="I89" s="49"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -5823,7 +5826,7 @@
       <c r="E90" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G90" s="97"/>
+      <c r="G90" s="94"/>
       <c r="I90" s="49"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -5835,7 +5838,7 @@
         <v>87</v>
       </c>
       <c r="F91" s="31"/>
-      <c r="G91" s="111"/>
+      <c r="G91" s="110"/>
       <c r="H91" s="17"/>
       <c r="I91" s="49"/>
     </row>
@@ -5942,7 +5945,7 @@
       <c r="F96" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="G96" s="111"/>
+      <c r="G96" s="110"/>
       <c r="H96" s="17"/>
       <c r="I96" s="49"/>
     </row>
@@ -5984,7 +5987,7 @@
       <c r="F98" s="32" t="s">
         <v>178</v>
       </c>
-      <c r="G98" s="114" t="s">
+      <c r="G98" s="111" t="s">
         <v>185</v>
       </c>
       <c r="H98" s="21"/>
@@ -5999,7 +6002,7 @@
         <v>116</v>
       </c>
       <c r="F99" s="31"/>
-      <c r="G99" s="115"/>
+      <c r="G99" s="112"/>
       <c r="H99" s="17"/>
       <c r="I99" s="49"/>
     </row>
@@ -6033,7 +6036,7 @@
       <c r="F101" s="32" t="s">
         <v>207</v>
       </c>
-      <c r="G101" s="97"/>
+      <c r="G101" s="94"/>
       <c r="I101" s="49"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -6044,7 +6047,7 @@
       <c r="F102" s="32" t="s">
         <v>205</v>
       </c>
-      <c r="G102" s="97"/>
+      <c r="G102" s="94"/>
       <c r="I102" s="49"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -6058,7 +6061,7 @@
       <c r="F103" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="G103" s="111"/>
+      <c r="G103" s="110"/>
       <c r="H103" s="17"/>
       <c r="I103" s="49"/>
     </row>
@@ -6184,6 +6187,9 @@
   </sheetData>
   <autoFilter ref="B2:H108" xr:uid="{6F42B86B-1E1B-4BC7-A1AC-69908067C16A}"/>
   <mergeCells count="17">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="G95:G96"/>
     <mergeCell ref="G100:G103"/>
     <mergeCell ref="G98:G99"/>
     <mergeCell ref="G4:G5"/>
@@ -6198,9 +6204,6 @@
     <mergeCell ref="G84:G91"/>
     <mergeCell ref="G40:G45"/>
     <mergeCell ref="G68:G80"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="G95:G96"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G68 G81:G108">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Optional">
@@ -6225,7 +6228,7 @@
   </sheetPr>
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" zoomScaleNormal="100" zoomScalePageLayoutView="88" workbookViewId="0">
+    <sheetView topLeftCell="A24" zoomScaleNormal="100" zoomScalePageLayoutView="88" workbookViewId="0">
       <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
@@ -6795,9 +6798,9 @@
   </sheetPr>
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -7088,16 +7091,28 @@
       </c>
     </row>
     <row r="10" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1">
+        <v>700</v>
+      </c>
+      <c r="E10" s="2">
+        <v>10</v>
+      </c>
       <c r="F10" s="3"/>
       <c r="G10" s="15"/>
       <c r="H10" s="1"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="1"/>
+      <c r="J10" s="1" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="11" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -7221,7 +7236,7 @@
   <dimension ref="A1:J8761"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -7259,6 +7274,9 @@
       <c r="H1" s="59" t="s">
         <v>336</v>
       </c>
+      <c r="I1" s="3" t="s">
+        <v>356</v>
+      </c>
       <c r="J1" s="59"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -7286,6 +7304,9 @@
       <c r="H2" s="3">
         <v>0.1</v>
       </c>
+      <c r="I2" s="3">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="88">
@@ -7312,6 +7333,9 @@
       <c r="H3" s="3">
         <v>0.1</v>
       </c>
+      <c r="I3" s="3">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="88">
@@ -7338,6 +7362,9 @@
       <c r="H4" s="3">
         <v>0.1</v>
       </c>
+      <c r="I4" s="3">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="88">
@@ -7364,6 +7391,9 @@
       <c r="H5" s="3">
         <v>0.1</v>
       </c>
+      <c r="I5" s="3">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="88">
@@ -7390,6 +7420,9 @@
       <c r="H6" s="3">
         <v>0.1</v>
       </c>
+      <c r="I6" s="3">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="88">
@@ -7416,6 +7449,9 @@
       <c r="H7" s="3">
         <v>0.1</v>
       </c>
+      <c r="I7" s="3">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="88">
@@ -7442,6 +7478,9 @@
       <c r="H8" s="3">
         <v>0.1</v>
       </c>
+      <c r="I8" s="3">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="88">
@@ -7468,6 +7507,9 @@
       <c r="H9" s="3">
         <v>0.3</v>
       </c>
+      <c r="I9" s="3">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="88">
@@ -7494,6 +7536,9 @@
       <c r="H10" s="3">
         <v>0.5</v>
       </c>
+      <c r="I10" s="3">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="88">
@@ -7520,6 +7565,9 @@
       <c r="H11" s="3">
         <v>0.7</v>
       </c>
+      <c r="I11" s="3">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="88">
@@ -7546,6 +7594,9 @@
       <c r="H12" s="3">
         <v>0.8</v>
       </c>
+      <c r="I12" s="3">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="88">
@@ -7572,6 +7623,9 @@
       <c r="H13" s="3">
         <v>0.8</v>
       </c>
+      <c r="I13" s="3">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="88">
@@ -7598,6 +7652,9 @@
       <c r="H14" s="3">
         <v>0.8</v>
       </c>
+      <c r="I14" s="3">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="88">
@@ -7624,6 +7681,9 @@
       <c r="H15" s="3">
         <v>0.3</v>
       </c>
+      <c r="I15" s="3">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="88">
@@ -7650,8 +7710,11 @@
       <c r="H16" s="3">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="88">
         <v>44927.625</v>
       </c>
@@ -7676,8 +7739,11 @@
       <c r="H17" s="3">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="88">
         <v>44927.666666666664</v>
       </c>
@@ -7702,8 +7768,11 @@
       <c r="H18" s="3">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="88">
         <v>44927.708333333336</v>
       </c>
@@ -7728,8 +7797,11 @@
       <c r="H19" s="3">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="88">
         <v>44927.75</v>
       </c>
@@ -7754,8 +7826,11 @@
       <c r="H20" s="3">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="88">
         <v>44927.791666666664</v>
       </c>
@@ -7780,8 +7855,11 @@
       <c r="H21" s="3">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="88">
         <v>44927.833333333336</v>
       </c>
@@ -7806,8 +7884,11 @@
       <c r="H22" s="3">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="88">
         <v>44927.875</v>
       </c>
@@ -7832,8 +7913,11 @@
       <c r="H23" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="88">
         <v>44927.916666666664</v>
       </c>
@@ -7858,8 +7942,11 @@
       <c r="H24" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="88">
         <v>44927.958333333336</v>
       </c>
@@ -7884,8 +7971,11 @@
       <c r="H25" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="88">
         <v>44928</v>
       </c>
@@ -7910,8 +8000,11 @@
       <c r="H26" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="88">
         <v>44928.041666666664</v>
       </c>
@@ -7936,8 +8029,11 @@
       <c r="H27" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="88">
         <v>44928.083333333336</v>
       </c>
@@ -7962,8 +8058,11 @@
       <c r="H28" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="88">
         <v>44928.125</v>
       </c>
@@ -7988,8 +8087,11 @@
       <c r="H29" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="88">
         <v>44928.166666666664</v>
       </c>
@@ -8014,8 +8116,11 @@
       <c r="H30" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="88">
         <v>44928.208333333336</v>
       </c>
@@ -8040,8 +8145,11 @@
       <c r="H31" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="88">
         <v>44928.25</v>
       </c>
@@ -8066,8 +8174,11 @@
       <c r="H32" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="88">
         <v>44928.291666666664</v>
       </c>
@@ -8092,8 +8203,11 @@
       <c r="H33" s="3">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="88">
         <v>44928.333333333336</v>
       </c>
@@ -8118,8 +8232,11 @@
       <c r="H34" s="3">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="88">
         <v>44928.375</v>
       </c>
@@ -8144,8 +8261,11 @@
       <c r="H35" s="3">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="88">
         <v>44928.416666666664</v>
       </c>
@@ -8170,8 +8290,11 @@
       <c r="H36" s="3">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="88">
         <v>44928.458333333336</v>
       </c>
@@ -8196,8 +8319,11 @@
       <c r="H37" s="3">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="88">
         <v>44928.5</v>
       </c>
@@ -8222,8 +8348,11 @@
       <c r="H38" s="3">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="88">
         <v>44928.541666666664</v>
       </c>
@@ -8248,8 +8377,11 @@
       <c r="H39" s="3">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="88">
         <v>44928.583333333336</v>
       </c>
@@ -8274,8 +8406,11 @@
       <c r="H40" s="3">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="88">
         <v>44928.625</v>
       </c>
@@ -8300,8 +8435,11 @@
       <c r="H41" s="3">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="88">
         <v>44928.666666666664</v>
       </c>
@@ -8326,8 +8464,11 @@
       <c r="H42" s="3">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="88">
         <v>44928.708333333336</v>
       </c>
@@ -8352,8 +8493,11 @@
       <c r="H43" s="3">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="88">
         <v>44928.75</v>
       </c>
@@ -8378,8 +8522,11 @@
       <c r="H44" s="3">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44" s="3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="88">
         <v>44928.791666666664</v>
       </c>
@@ -8404,8 +8551,11 @@
       <c r="H45" s="3">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" s="3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="88">
         <v>44928.833333333336</v>
       </c>
@@ -8430,8 +8580,11 @@
       <c r="H46" s="3">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="88">
         <v>44928.875</v>
       </c>
@@ -8456,8 +8609,11 @@
       <c r="H47" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="88">
         <v>44928.916666666664</v>
       </c>
@@ -8482,8 +8638,11 @@
       <c r="H48" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="88">
         <v>44928.958333333336</v>
       </c>
@@ -8508,8 +8667,11 @@
       <c r="H49" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="88">
         <v>44929</v>
       </c>
@@ -8517,7 +8679,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="88">
         <v>44929.041666666664</v>
       </c>
@@ -8525,7 +8687,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="88">
         <v>44929.083333333336</v>
       </c>
@@ -8533,7 +8695,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="88">
         <v>44929.125</v>
       </c>
@@ -8541,7 +8703,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="88">
         <v>44929.166666666664</v>
       </c>
@@ -8549,7 +8711,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="88">
         <v>44929.208333333336</v>
       </c>
@@ -8557,7 +8719,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="88">
         <v>44929.25</v>
       </c>
@@ -8565,7 +8727,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="88">
         <v>44929.291666666664</v>
       </c>
@@ -8573,7 +8735,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="88">
         <v>44929.333333333336</v>
       </c>
@@ -8581,7 +8743,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="88">
         <v>44929.375</v>
       </c>
@@ -8589,7 +8751,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="88">
         <v>44929.416666666664</v>
       </c>
@@ -8597,7 +8759,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="88">
         <v>44929.458333333336</v>
       </c>
@@ -8605,7 +8767,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="88">
         <v>44929.5</v>
       </c>
@@ -8613,7 +8775,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="88">
         <v>44929.541666666664</v>
       </c>
@@ -8621,7 +8783,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="88">
         <v>44929.583333333336</v>
       </c>
@@ -78657,7 +78819,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.69921875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -78791,9 +78953,15 @@
       <c r="D10" s="9"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="1"/>
+      <c r="A11" s="8">
+        <v>2</v>
+      </c>
+      <c r="B11" s="8">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1">
+        <v>10</v>
+      </c>
       <c r="D11" s="9"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -79121,14 +79289,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2eb1e4af-f854-4f79-85c1-6f26940025e4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d4a0f758-4b96-4ff5-8d06-f95a3d3dda1e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -79381,29 +79547,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2eb1e4af-f854-4f79-85c1-6f26940025e4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d4a0f758-4b96-4ff5-8d06-f95a3d3dda1e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D351F7AA-766C-4547-802C-9F4B7AB5F83E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80A89352-0353-48F1-9429-0E3BD72B2E30}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a656bf76-cca4-4796-b3e3-9ff4debad9ca"/>
-    <ds:schemaRef ds:uri="3f4d043c-ef99-408b-9086-307465b47223"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="2eb1e4af-f854-4f79-85c1-6f26940025e4"/>
-    <ds:schemaRef ds:uri="d4a0f758-4b96-4ff5-8d06-f95a3d3dda1e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -79428,9 +79585,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80A89352-0353-48F1-9429-0E3BD72B2E30}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D351F7AA-766C-4547-802C-9F4B7AB5F83E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a656bf76-cca4-4796-b3e3-9ff4debad9ca"/>
+    <ds:schemaRef ds:uri="3f4d043c-ef99-408b-9086-307465b47223"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="2eb1e4af-f854-4f79-85c1-6f26940025e4"/>
+    <ds:schemaRef ds:uri="d4a0f758-4b96-4ff5-8d06-f95a3d3dda1e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>